<commit_message>
Fix export tests formatting changes, part 2
</commit_message>
<xml_diff>
--- a/jems-ui/e2e/cypress/fixtures/project/exports/partners-budget/TB-369-export-de-en.xlsx
+++ b/jems-ui/e2e/cypress/fixtures/project/exports/partners-budget/TB-369-export-de-en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jems\ems\jems-ui\e2e\cypress\downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jems\ems\jems-ui\e2e\cypress\fixtures\project\exports\partners-budget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59969A7A-75E4-4E58-97ED-0F5691E0BD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D60701-E7C5-42AB-9272-746FD4270E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31740" yWindow="2175" windowWidth="32100" windowHeight="17910" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="first_tab" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="99">
   <si>
     <t>D - Project budget</t>
   </si>
@@ -275,9 +275,6 @@
     <t>External expertise and services</t>
   </si>
   <si>
-    <t>API generated travel and accommodation cost award procedures EN</t>
-  </si>
-  <si>
     <t>Equipment</t>
   </si>
   <si>
@@ -309,6 +306,18 @@
   </si>
   <si>
     <t>Preparation Lump sum EN</t>
+  </si>
+  <si>
+    <t>API generated external cost description EN</t>
+  </si>
+  <si>
+    <t>API generated external cost comments EN</t>
+  </si>
+  <si>
+    <t>API generated external cost award procedures EN</t>
+  </si>
+  <si>
+    <t>API generated external cost unit type EN</t>
   </si>
 </sst>
 </file>
@@ -1451,8 +1460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1796,13 +1805,13 @@
         <v>83</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>31</v>
@@ -1817,7 +1826,7 @@
         <v>78</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="R6" s="6">
         <v>1</v>
@@ -1885,16 +1894,16 @@
         <v>29</v>
       </c>
       <c r="I7" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="L7" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>31</v>
@@ -1909,7 +1918,7 @@
         <v>78</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R7" s="6">
         <v>5</v>
@@ -1977,16 +1986,16 @@
         <v>29</v>
       </c>
       <c r="I8" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="K8" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="L8" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>93</v>
       </c>
       <c r="M8" s="5" t="s">
         <v>31</v>
@@ -2001,7 +2010,7 @@
         <v>78</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R8" s="6">
         <v>5.5</v>
@@ -2164,7 +2173,7 @@
         <v>53</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>31</v>
@@ -2176,7 +2185,7 @@
         <v>31</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O10" s="5">
         <v>0</v>

</xml_diff>